<commit_message>
update pivot filter and config fonts
</commit_message>
<xml_diff>
--- a/english/net/developer-guide/pivot-tables/add-filter-in-pivot-table/filterout.xlsx
+++ b/english/net/developer-guide/pivot-tables/add-filter-in-pivot-table/filterout.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Fruit</t>
   </si>
@@ -50,20 +51,28 @@
     <t>Sum of Count</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Evaluation Only. Created with Aspose.Cells for .NET. Copyright 2003 - 2024 Aspose Pty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -158,9 +167,13 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
@@ -173,6 +186,10 @@
       <protection/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
@@ -303,7 +320,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="3" refreshOnLoad="1" refreshedBy="Aspose" refreshedDate="44743.5711677611" recordCount="7">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Aspose" refreshedDate="45645.4097740809" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="7">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:B8" sheet="Sheet1"/>
   </cacheSource>
@@ -320,14 +337,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Count">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" count="6">
-        <n v="5"/>
-        <n v="3"/>
-        <n v="6"/>
-        <n v="4"/>
-        <n v="2"/>
-        <n v="20"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1"/>
     </cacheField>
   </cacheFields>
 </pivotCacheDefinition>
@@ -337,40 +347,40 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="7">
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="1"/>
+    <n v="3"/>
   </r>
   <r>
     <x v="2"/>
-    <x v="2"/>
+    <n v="6"/>
   </r>
   <r>
     <x v="3"/>
-    <x v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="4"/>
-    <x v="0"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="5"/>
-    <x v="4"/>
+    <n v="2"/>
   </r>
   <r>
     <x v="6"/>
-    <x v="5"/>
+    <n v="20"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" showMissing="1" preserveFormatting="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="1" showMemberPropertyTips="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" compact="0" compactData="0">
   <location ref="D10:E16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
-    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" sortType="descending">
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1" sortType="descending">
       <items count="8">
         <item x="0"/>
         <item x="1"/>
@@ -382,35 +392,35 @@
         <item t="default"/>
       </items>
       <autoSortScope>
-        <pivotArea outline="0" fieldPosition="0" type="normal">
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
           <references count="1">
-            <reference field="4294967294" count="1">
+            <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
             </reference>
           </references>
         </pivotArea>
       </autoSortScope>
     </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
   <rowItems count="6">
     <i>
-      <x v="2"/>
+      <x/>
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i>
-      <x/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -424,10 +434,10 @@
   </dataFields>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="0" type="count" evalOrder="-1" id="0" iMeasureFld="0" stringValue1="5">
+    <filter fld="0" type="count" id="0" iMeasureFld="0">
       <autoFilter ref="A1">
         <filterColumn colId="0">
-          <top10 val="5"/>
+          <top10 top="0" val="5"/>
         </filterColumn>
       </autoFilter>
     </filter>
@@ -731,14 +741,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53151eaf-463a-4ea9-ae27-c3bb3e3b3006}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64bd0e40-aaac-4a46-b2c4-fc0f34900395}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="13.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="10.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -808,58 +818,76 @@
     </row>
     <row r="10" spans="4:5" ht="12.75">
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="4:5" ht="12.75">
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="12.75">
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="12.75">
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
         <v>4</v>
       </c>
-      <c r="E11" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5" ht="12.75">
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" ht="12.75">
-      <c r="D13" s="3" t="s">
+    </row>
+    <row r="14" spans="4:5" ht="12.75">
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="12.75">
+      <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5">
         <v>2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" ht="12.75">
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" ht="12.75">
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4">
-        <v>3</v>
       </c>
     </row>
     <row r="16" spans="4:5" ht="12.75">
       <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34e18439-69fb-48bd-be40-341de7f27545}">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="5" spans="1:1" ht="23.25" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E16" s="1">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>